<commit_message>
Created Folder Check and Split PDF Sequence.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GreatBots\Documents\UiPath\IACET_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +84,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -159,13 +155,97 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>InsuranceIacetProcessingPDFDailyCase</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>IACET_Performer_March_2024</t>
+  </si>
+  <si>
+    <t>IACET</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>InputFiles</t>
+  </si>
+  <si>
+    <t>OutputFiles</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>ERDT</t>
+  </si>
+  <si>
+    <t>C:\Users\GreatBots\Documents\UiPath\IACET_Performer\Data\Input\IACET DATA.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\GreatBots\Documents\UiPath\IACET_Performer\Data\Input\Policy Details.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\GreatBots\Documents\UiPath\IACET_Performer\Data\Output</t>
+  </si>
+  <si>
+    <t>C:\Users\GreatBots\Documents\UiPath\IACET_Performer\Data\PDF Reporting Template.xlsx</t>
+  </si>
+  <si>
+    <t>ReportingTemplate</t>
+  </si>
+  <si>
+    <t>IacetData</t>
+  </si>
+  <si>
+    <t>PolicyDetails</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>SupportEmail</t>
+  </si>
+  <si>
+    <t>SupportSubject</t>
+  </si>
+  <si>
+    <t>SupportBody</t>
+  </si>
+  <si>
+    <t>IsSupportEmailSend</t>
+  </si>
+  <si>
+    <t>IsEmailSend</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>SheetCountryDetails</t>
+  </si>
+  <si>
+    <t>SheetPolicyType</t>
+  </si>
+  <si>
+    <t>Sheet3</t>
+  </si>
+  <si>
+    <t>SheetInfo</t>
+  </si>
+  <si>
+    <t>Temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -191,12 +271,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -211,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,6 +307,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,19 +621,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" customWidth="1"/>
+    <col min="3" max="3" width="99" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -559,7 +647,9 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -585,63 +675,259 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"{"&amp;""""&amp; A2 &amp; """"&amp; ","&amp;""""&amp;B2&amp; """"&amp; "}"</f>
+        <v>{"OrchestratorQueueName","InsuranceIacetProcessingPDFDailyCase"}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="45">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D23" si="0">"{"&amp;""""&amp; A3 &amp; """"&amp; ","&amp;""""&amp;B3&amp; """"&amp; "}"</f>
+        <v>{"OrchestratorQueueFolder","Shared"}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>{"ERDT",""}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IACET",""}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="30">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{"logF_BusinessProcessName","IACET_Performer_March_2024"}</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
+    <row r="7" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{"Email",""}</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IsEmailSend",""}</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>{"Subject",""}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>{"Body",""}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>{"",""}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>{"SupportEmail",""}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>{"SupportSubject",""}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>{"SupportBody",""}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IsSupportEmailSend",""}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>{"",""}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>{"InputFiles",""}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>{"IacetData","C:\Users\GreatBots\Documents\UiPath\IACET_Performer\Data\Input\IACET DATA.xlsx"}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>{"SheetInfo","Sheet1"}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>{"PolicyDetails","C:\Users\GreatBots\Documents\UiPath\IACET_Performer\Data\Input\Policy Details.xlsx"}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>{"SheetCountryDetails","Sheet1"}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>{"SheetPolicyType","Sheet3"}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>{"",""}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1608,6 +1894,13 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1616,19 +1909,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1958,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1673,18 +1966,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +2001,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +2023,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +2034,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +2045,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2779,17 +3072,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +3093,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>